<commit_message>
Started working on cell data sheet as far as setting up the structure. Things that need to be done: 1) outline sections 2) remove all color from diagrams 3) assign any descriptions to be completed by their designer.
</commit_message>
<xml_diff>
--- a/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
+++ b/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -101,8 +104,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,7 +411,7 @@
   <dimension ref="D3:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added all pictures required for Cell data sheet
</commit_message>
<xml_diff>
--- a/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
+++ b/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -36,6 +36,42 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>SRAM WE</t>
+  </si>
+  <si>
+    <t>SRAM OE</t>
+  </si>
+  <si>
+    <t>SRAM CE</t>
+  </si>
+  <si>
+    <t>ADDR &lt;14&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;15&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;13&gt;</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>ADDR &lt;12&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;11&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;10&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;9&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;8&gt;</t>
   </si>
 </sst>
 </file>
@@ -411,12 +447,12 @@
   <dimension ref="D3:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -433,84 +469,108 @@
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E6" s="2">
         <v>3</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E7" s="2">
         <v>4</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" s="2">
         <v>5</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E9" s="2">
         <v>6</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E10" s="2">
         <v>7</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E11" s="2">
         <v>8</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E12" s="2">
         <v>9</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E13" s="2">
         <v>10</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E14" s="2">
         <v>11</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E15" s="2">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
seperated timing data, added timing data to all completed cell data sheets,
</commit_message>
<xml_diff>
--- a/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
+++ b/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -72,6 +72,210 @@
   </si>
   <si>
     <t>ADDR &lt;8&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;7&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;6&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;5&gt;</t>
+  </si>
+  <si>
+    <t>VDD</t>
+  </si>
+  <si>
+    <t>ADDR &lt;4&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;3&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;2&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>ADDR &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;2&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;3&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;4&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;6&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;8&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;9&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;10&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;11&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;12&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;13&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;14&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;5&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;7&gt;</t>
+  </si>
+  <si>
+    <t>DIN &lt;15&gt;</t>
+  </si>
+  <si>
+    <t>ROM_CE</t>
+  </si>
+  <si>
+    <t>ROM_OE</t>
+  </si>
+  <si>
+    <t>RGB &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>RGB &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>hSync</t>
+  </si>
+  <si>
+    <t>vSync</t>
+  </si>
+  <si>
+    <t>PSR &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>PSR &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>PSR &lt;3&gt;</t>
+  </si>
+  <si>
+    <t>PSR &lt;2&gt;</t>
+  </si>
+  <si>
+    <t>PSR &lt;4&gt;</t>
+  </si>
+  <si>
+    <t>CTRLR LATCH &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>CTRLR LATCH &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>CTRLR DATA &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>CTRLR DATA &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>CLK PI;SE</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>STATE BIT</t>
+  </si>
+  <si>
+    <t>AUDIO DAC &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>AUDIO DAC &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>AUDIO DAC &lt;2&gt;</t>
+  </si>
+  <si>
+    <t>AUDIO DAC &lt;3&gt;</t>
+  </si>
+  <si>
+    <t>AUDIO_ROM_SPI_MISO</t>
+  </si>
+  <si>
+    <t>AUDIO_ROM_SPI_MOSI</t>
+  </si>
+  <si>
+    <t>AUDIO_ROM_SPI_CLK</t>
+  </si>
+  <si>
+    <t>AUDIO_ROM_SPI_CE</t>
+  </si>
+  <si>
+    <t>DOUT &lt;15&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;14&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;13&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;12&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;11&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;10&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;9&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;8&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;7&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;6&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;5&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;4&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;3&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;2&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>DOUT &lt;0&gt;</t>
   </si>
 </sst>
 </file>
@@ -101,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,16 +328,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,13 +664,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -577,504 +795,648 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="E16" s="2">
         <v>13</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E17" s="2">
         <v>14</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E18" s="2">
         <v>15</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E19" s="2">
         <v>16</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E20" s="2">
         <v>17</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E21" s="2">
         <v>18</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E22" s="2">
         <v>19</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E23" s="2">
         <v>20</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E24" s="2">
         <v>21</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E25" s="2">
         <v>22</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E26" s="2">
         <v>23</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E27" s="2">
         <v>24</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E28" s="2">
         <v>25</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E29" s="2">
         <v>26</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E30" s="2">
         <v>27</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E31" s="2">
         <v>28</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D32" s="2"/>
+      <c r="D32" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="E32" s="2">
         <v>29</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E33" s="2">
         <v>30</v>
       </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E34" s="2">
         <v>31</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E35" s="2">
         <v>32</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E36" s="2">
         <v>33</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E37" s="2">
         <v>34</v>
       </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E38" s="2">
         <v>35</v>
       </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E39" s="2">
         <v>36</v>
       </c>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="E40" s="2">
         <v>37</v>
       </c>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E41" s="2">
         <v>38</v>
       </c>
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E42" s="2">
         <v>39</v>
       </c>
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E43" s="2">
         <v>40</v>
       </c>
       <c r="F43" s="2"/>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E44" s="2">
         <v>41</v>
       </c>
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E45" s="2">
         <v>42</v>
       </c>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E46" s="2">
         <v>43</v>
       </c>
       <c r="F46" s="2"/>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E47" s="2">
         <v>44</v>
       </c>
       <c r="F47" s="2"/>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E48" s="2">
         <v>45</v>
       </c>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E49" s="2">
         <v>46</v>
       </c>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D50" s="2"/>
+      <c r="D50" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E50" s="2">
         <v>47</v>
       </c>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E51" s="2">
         <v>48</v>
       </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E52" s="2">
         <v>49</v>
       </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E53" s="2">
         <v>50</v>
       </c>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E54" s="2">
         <v>51</v>
       </c>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E55" s="2">
         <v>52</v>
       </c>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="E56" s="2">
         <v>53</v>
       </c>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="E57" s="2">
         <v>54</v>
       </c>
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E58" s="2">
         <v>55</v>
       </c>
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E59" s="2">
         <v>56</v>
       </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E60" s="2">
         <v>57</v>
       </c>
       <c r="F60" s="2"/>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E61" s="2">
         <v>58</v>
       </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="E62" s="2">
         <v>59</v>
       </c>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="E63" s="2">
         <v>60</v>
       </c>
       <c r="F63" s="2"/>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D64" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E64" s="2">
         <v>61</v>
       </c>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D65" s="2"/>
+      <c r="D65" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="E65" s="2">
         <v>62</v>
       </c>
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="E66" s="2">
         <v>63</v>
       </c>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="E67" s="2">
         <v>64</v>
       </c>
       <c r="F67" s="2"/>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D68" s="2"/>
+      <c r="D68" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="E68" s="2">
         <v>65</v>
       </c>
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D69" s="2"/>
+      <c r="D69" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E69" s="2">
         <v>66</v>
       </c>
       <c r="F69" s="2"/>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D70" s="2"/>
+      <c r="D70" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E70" s="2">
         <v>67</v>
       </c>
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="E71" s="2">
         <v>68</v>
       </c>
       <c r="F71" s="2"/>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D72" s="2"/>
+      <c r="D72" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E72" s="2">
         <v>69</v>
       </c>
       <c r="F72" s="2"/>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D73" s="2"/>
+      <c r="D73" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E73" s="2">
         <v>70</v>
       </c>
       <c r="F73" s="2"/>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D74" s="2"/>
+      <c r="D74" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E74" s="2">
         <v>71</v>
       </c>
       <c r="F74" s="2"/>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D75" s="2"/>
+      <c r="D75" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E75" s="2">
         <v>72</v>
       </c>
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D76" s="2"/>
+      <c r="D76" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E76" s="2">
         <v>73</v>
       </c>
       <c r="F76" s="2"/>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E77" s="2">
         <v>74</v>
       </c>
       <c r="F77" s="2"/>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D78" s="2"/>
+      <c r="D78" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="E78" s="2">
         <v>75</v>
       </c>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D79" s="2"/>
+      <c r="D79" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E79" s="2">
         <v>76</v>
       </c>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E80" s="2">
         <v>77</v>
       </c>
       <c r="F80" s="2"/>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D81" s="2"/>
+      <c r="D81" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E81" s="2">
         <v>78</v>
       </c>
       <c r="F81" s="2"/>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D82" s="2"/>
+      <c r="D82" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="E82" s="2">
         <v>79</v>
       </c>
       <c r="F82" s="2"/>
     </row>
     <row r="83" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D83" s="2"/>
+      <c r="D83" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E83" s="2">
         <v>80</v>
       </c>
       <c r="F83" s="2"/>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D84" s="2"/>
+      <c r="D84" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E84" s="2">
         <v>81</v>
       </c>
       <c r="F84" s="2"/>
     </row>
     <row r="85" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D85" s="2"/>
+      <c r="D85" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E85" s="2">
         <v>82</v>
       </c>
       <c r="F85" s="2"/>
     </row>
     <row r="86" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D86" s="2"/>
+      <c r="D86" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="E86" s="2">
         <v>83</v>
       </c>
       <c r="F86" s="2"/>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D87" s="2"/>
+      <c r="D87" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="E87" s="2">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Updated chip data sheet, pin table, added abreviations table
</commit_message>
<xml_diff>
--- a/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
+++ b/Documents/Final Documentation/Chip Data Sheet/PinOutTable.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -188,15 +188,6 @@
     <t>CTRLR LATCH &lt;0&gt;</t>
   </si>
   <si>
-    <t>CTRLR DATA &lt;1&gt;</t>
-  </si>
-  <si>
-    <t>CTRLR DATA &lt;0&gt;</t>
-  </si>
-  <si>
-    <t>CLK PI;SE</t>
-  </si>
-  <si>
     <t>NC</t>
   </si>
   <si>
@@ -276,6 +267,255 @@
   </si>
   <si>
     <t>DOUT &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>Not Connected</t>
+  </si>
+  <si>
+    <t>SRAM Write Enable</t>
+  </si>
+  <si>
+    <t>SRAM Output Enabale</t>
+  </si>
+  <si>
+    <t>SRAM Chip Enable</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Digital Power Supply</t>
+  </si>
+  <si>
+    <t>Clock Input</t>
+  </si>
+  <si>
+    <t>Address Bit-15 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-14 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-13 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-12 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-11 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-10 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-9 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-8 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-7 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-6 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-5 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-4 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-3 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-2 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-1 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Address Bit-0 connected to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-0 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-1 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-2 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-3 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-4 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>CTRLR Data in &lt;1&gt;</t>
+  </si>
+  <si>
+    <t>CTRLR Data in &lt;0&gt;</t>
+  </si>
+  <si>
+    <t>Data in Bit-5 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-7 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-8 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-9 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-10 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-11 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-12 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-13 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-14 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-15 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>Data in Bit-6 connect to both SRAM and ROM</t>
+  </si>
+  <si>
+    <t>ROM Chip Enable</t>
+  </si>
+  <si>
+    <t>ROM Output Enable</t>
+  </si>
+  <si>
+    <t>Horizontal Sync required for VGA</t>
+  </si>
+  <si>
+    <t>Vertical Sync required for VGA</t>
+  </si>
+  <si>
+    <t>Least Significant Bit for VGA Color</t>
+  </si>
+  <si>
+    <t>Most Significant Bit for VGA Color</t>
+  </si>
+  <si>
+    <t>Program Status Register Bit-0 used for Debugging</t>
+  </si>
+  <si>
+    <t>Program Status Register Bit-1 used for Debugging</t>
+  </si>
+  <si>
+    <t>Program Status Register Bit-2 used for Debugging</t>
+  </si>
+  <si>
+    <t>Program Status Register Bit-3 used for Debugging</t>
+  </si>
+  <si>
+    <t>Program Status Register Bit-4 used for Debugging</t>
+  </si>
+  <si>
+    <t>CLK PULSE</t>
+  </si>
+  <si>
+    <t>Clock Output to Both Controllers</t>
+  </si>
+  <si>
+    <t>Controler 2 Latch signal</t>
+  </si>
+  <si>
+    <t>Controler 1 Latch signal</t>
+  </si>
+  <si>
+    <t>Controler 2 Data Signal</t>
+  </si>
+  <si>
+    <t>Controler 1 Data Signal</t>
+  </si>
+  <si>
+    <t>Program State Bit used for Debugging</t>
+  </si>
+  <si>
+    <t>Audio rom SPI Clock</t>
+  </si>
+  <si>
+    <t>Audio Rom SPI Chip Enable</t>
+  </si>
+  <si>
+    <t>Audio ROM SPI Master out Slave in</t>
+  </si>
+  <si>
+    <t>Audio ROM SPI Master in Slave out</t>
+  </si>
+  <si>
+    <t>Data out Bit-15 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-14 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-13 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-12 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-11 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-10 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-9 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-8 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-7 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-6 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-5 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-4 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-3 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-2 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-1 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Data out Bit-0 Connected to SRAM Only</t>
+  </si>
+  <si>
+    <t>Audio DAC Output Bit-0</t>
+  </si>
+  <si>
+    <t>Audio DAC Output Bit-1</t>
+  </si>
+  <si>
+    <t>Audio DAC Output Bit-2</t>
+  </si>
+  <si>
+    <t>Audio DAC Output Bit-3</t>
   </si>
 </sst>
 </file>
@@ -664,15 +904,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:6" x14ac:dyDescent="0.3">
@@ -693,7 +933,9 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D5" s="2" t="s">
@@ -702,7 +944,9 @@
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
@@ -711,7 +955,9 @@
       <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
@@ -720,7 +966,9 @@
       <c r="E7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
@@ -729,7 +977,9 @@
       <c r="E8" s="2">
         <v>5</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
@@ -738,7 +988,9 @@
       <c r="E9" s="2">
         <v>6</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
@@ -747,7 +999,9 @@
       <c r="E10" s="2">
         <v>7</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
@@ -756,7 +1010,9 @@
       <c r="E11" s="2">
         <v>8</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
@@ -765,7 +1021,9 @@
       <c r="E12" s="2">
         <v>9</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="13" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
@@ -774,7 +1032,9 @@
       <c r="E13" s="2">
         <v>10</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
@@ -783,7 +1043,9 @@
       <c r="E14" s="2">
         <v>11</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
@@ -792,7 +1054,9 @@
       <c r="E15" s="2">
         <v>12</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D16" s="2" t="s">
@@ -801,7 +1065,9 @@
       <c r="E16" s="2">
         <v>13</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
@@ -810,7 +1076,9 @@
       <c r="E17" s="2">
         <v>14</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
@@ -819,7 +1087,9 @@
       <c r="E18" s="2">
         <v>15</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
@@ -828,7 +1098,9 @@
       <c r="E19" s="2">
         <v>16</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
@@ -837,7 +1109,9 @@
       <c r="E20" s="2">
         <v>17</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
@@ -846,7 +1120,9 @@
       <c r="E21" s="2">
         <v>18</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
@@ -855,7 +1131,9 @@
       <c r="E22" s="2">
         <v>19</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" s="2" t="s">
@@ -864,7 +1142,9 @@
       <c r="E23" s="2">
         <v>20</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D24" s="2" t="s">
@@ -873,7 +1153,9 @@
       <c r="E24" s="2">
         <v>21</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D25" s="2" t="s">
@@ -882,7 +1164,9 @@
       <c r="E25" s="2">
         <v>22</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D26" s="2" t="s">
@@ -891,7 +1175,9 @@
       <c r="E26" s="2">
         <v>23</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D27" s="2" t="s">
@@ -900,7 +1186,9 @@
       <c r="E27" s="2">
         <v>24</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D28" s="2" t="s">
@@ -909,7 +1197,9 @@
       <c r="E28" s="2">
         <v>25</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D29" s="2" t="s">
@@ -918,7 +1208,9 @@
       <c r="E29" s="2">
         <v>26</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D30" s="2" t="s">
@@ -927,7 +1219,9 @@
       <c r="E30" s="2">
         <v>27</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D31" s="2" t="s">
@@ -936,7 +1230,9 @@
       <c r="E31" s="2">
         <v>28</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D32" s="3" t="s">
@@ -945,7 +1241,9 @@
       <c r="E32" s="2">
         <v>29</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D33" s="2" t="s">
@@ -954,7 +1252,9 @@
       <c r="E33" s="2">
         <v>30</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
@@ -963,7 +1263,9 @@
       <c r="E34" s="2">
         <v>31</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D35" s="2" t="s">
@@ -972,7 +1274,9 @@
       <c r="E35" s="2">
         <v>32</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D36" s="2" t="s">
@@ -981,7 +1285,9 @@
       <c r="E36" s="2">
         <v>33</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D37" s="2" t="s">
@@ -990,7 +1296,9 @@
       <c r="E37" s="2">
         <v>34</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D38" s="2" t="s">
@@ -999,7 +1307,9 @@
       <c r="E38" s="2">
         <v>35</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D39" s="2" t="s">
@@ -1008,7 +1318,9 @@
       <c r="E39" s="2">
         <v>36</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D40" s="2" t="s">
@@ -1017,7 +1329,9 @@
       <c r="E40" s="2">
         <v>37</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D41" s="2" t="s">
@@ -1026,7 +1340,9 @@
       <c r="E41" s="2">
         <v>38</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D42" s="2" t="s">
@@ -1035,7 +1351,9 @@
       <c r="E42" s="2">
         <v>39</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D43" s="2" t="s">
@@ -1044,7 +1362,9 @@
       <c r="E43" s="2">
         <v>40</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D44" s="2" t="s">
@@ -1053,7 +1373,9 @@
       <c r="E44" s="2">
         <v>41</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D45" s="2" t="s">
@@ -1062,7 +1384,9 @@
       <c r="E45" s="2">
         <v>42</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D46" s="2" t="s">
@@ -1071,7 +1395,9 @@
       <c r="E46" s="2">
         <v>43</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D47" s="2" t="s">
@@ -1080,7 +1406,9 @@
       <c r="E47" s="2">
         <v>44</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D48" s="2" t="s">
@@ -1089,7 +1417,9 @@
       <c r="E48" s="2">
         <v>45</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D49" s="2" t="s">
@@ -1098,7 +1428,9 @@
       <c r="E49" s="2">
         <v>46</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D50" s="2" t="s">
@@ -1107,7 +1439,9 @@
       <c r="E50" s="2">
         <v>47</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D51" s="2" t="s">
@@ -1116,7 +1450,9 @@
       <c r="E51" s="2">
         <v>48</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D52" s="2" t="s">
@@ -1125,7 +1461,9 @@
       <c r="E52" s="2">
         <v>49</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D53" s="2" t="s">
@@ -1134,7 +1472,9 @@
       <c r="E53" s="2">
         <v>50</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D54" s="2" t="s">
@@ -1143,7 +1483,9 @@
       <c r="E54" s="2">
         <v>51</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D55" s="2" t="s">
@@ -1152,43 +1494,53 @@
       <c r="E55" s="2">
         <v>52</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D56" s="2" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="E56" s="2">
         <v>53</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D57" s="2" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="E57" s="2">
         <v>54</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="2" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D58" s="2" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="E58" s="2">
         <v>55</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D59" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E59" s="2">
         <v>56</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D60" s="2" t="s">
@@ -1197,151 +1549,185 @@
       <c r="E60" s="2">
         <v>57</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D61" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E61" s="2">
         <v>58</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D62" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E62" s="2">
         <v>59</v>
       </c>
-      <c r="F62" s="2"/>
+      <c r="F62" s="2" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D63" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E63" s="2">
         <v>60</v>
       </c>
-      <c r="F63" s="2"/>
+      <c r="F63" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D64" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E64" s="2">
         <v>61</v>
       </c>
-      <c r="F64" s="2"/>
+      <c r="F64" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D65" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E65" s="2">
         <v>62</v>
       </c>
-      <c r="F65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D66" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E66" s="2">
         <v>63</v>
       </c>
-      <c r="F66" s="2"/>
+      <c r="F66" s="2" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D67" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E67" s="2">
         <v>64</v>
       </c>
-      <c r="F67" s="2"/>
+      <c r="F67" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D68" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E68" s="2">
         <v>65</v>
       </c>
-      <c r="F68" s="2"/>
+      <c r="F68" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D69" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E69" s="2">
         <v>66</v>
       </c>
-      <c r="F69" s="2"/>
+      <c r="F69" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D70" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E70" s="2">
         <v>67</v>
       </c>
-      <c r="F70" s="2"/>
+      <c r="F70" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D71" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E71" s="2">
         <v>68</v>
       </c>
-      <c r="F71" s="2"/>
+      <c r="F71" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D72" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E72" s="2">
         <v>69</v>
       </c>
-      <c r="F72" s="2"/>
+      <c r="F72" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D73" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E73" s="2">
         <v>70</v>
       </c>
-      <c r="F73" s="2"/>
+      <c r="F73" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D74" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E74" s="2">
         <v>71</v>
       </c>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D75" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E75" s="2">
         <v>72</v>
       </c>
-      <c r="F75" s="2"/>
+      <c r="F75" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D76" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E76" s="2">
         <v>73</v>
       </c>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D77" s="2" t="s">
@@ -1350,97 +1736,119 @@
       <c r="E77" s="2">
         <v>74</v>
       </c>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D78" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E78" s="2">
         <v>75</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D79" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E79" s="2">
         <v>76</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D80" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E80" s="2">
         <v>77</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D81" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E81" s="2">
         <v>78</v>
       </c>
-      <c r="F81" s="2"/>
+      <c r="F81" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D82" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E82" s="2">
         <v>79</v>
       </c>
-      <c r="F82" s="2"/>
+      <c r="F82" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="83" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D83" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E83" s="2">
         <v>80</v>
       </c>
-      <c r="F83" s="2"/>
+      <c r="F83" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D84" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E84" s="2">
         <v>81</v>
       </c>
-      <c r="F84" s="2"/>
+      <c r="F84" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="85" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D85" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E85" s="2">
         <v>82</v>
       </c>
-      <c r="F85" s="2"/>
+      <c r="F85" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="86" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D86" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E86" s="2">
         <v>83</v>
       </c>
-      <c r="F86" s="2"/>
+      <c r="F86" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D87" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E87" s="2">
         <v>84</v>
       </c>
-      <c r="F87" s="2"/>
+      <c r="F87" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>